<commit_message>
Trial run with config file
</commit_message>
<xml_diff>
--- a/input/Config.xlsx
+++ b/input/Config.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0F1B4DD-6778-4E6C-B29E-446501529D7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -66,7 +67,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -377,21 +378,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="51.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="51.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -402,18 +403,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -424,34 +425,34 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>13</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Fix ResetBrowser / Update GetRecommended7 comment / Testing GetRecommended8
</commit_message>
<xml_diff>
--- a/input/Config.xlsx
+++ b/input/Config.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A90F5512-E27D-497A-B327-474E041B9CD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10296"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -67,7 +66,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -378,21 +377,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="51.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="51.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -403,7 +402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -414,7 +413,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -425,18 +424,18 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -447,7 +446,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
GetRecommended8 - merged version 6 and 7 into one XAML
</commit_message>
<xml_diff>
--- a/input/Config.xlsx
+++ b/input/Config.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t>Description</t>
   </si>
@@ -61,6 +61,12 @@
   </si>
   <si>
     <t>NumberOfPages</t>
+  </si>
+  <si>
+    <t>FormatWordReport</t>
+  </si>
+  <si>
+    <t>Yes - Format paragraphs into table</t>
   </si>
 </sst>
 </file>
@@ -378,10 +384,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -429,7 +435,7 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
@@ -455,6 +461,17 @@
       </c>
       <c r="C6" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>